<commit_message>
Se calcula el tiempo de ejecución. Se optimiza la búsqueda de un profesor para el curso generando un break al encontrar el profesor
</commit_message>
<xml_diff>
--- a/input/cursos.xlsx
+++ b/input/cursos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacLeod/Playground/chorario/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8327DC-4BE8-FF4A-8D33-1AD98962663F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E71D97F-94AF-D249-8902-96DA3A47E366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$268</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -902,17 +902,9 @@
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.33203125" customWidth="1"/>
-    <col min="13" max="13" width="1.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>